<commit_message>
Fix error handling and display detailed error messages
</commit_message>
<xml_diff>
--- a/public/template/EmployeeProfile_Template.xlsx
+++ b/public/template/EmployeeProfile_Template.xlsx
@@ -2,26 +2,45 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\Template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB80564-D212-44F7-A0BD-74178CF42F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2985D16-1775-4992-B532-7D17F4788256}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{48DF0B5B-2EB1-48FA-B103-CF6083A81732}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
     <t>Last Name</t>
   </si>
   <si>
@@ -59,9 +78,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>Employee ID</t>
   </si>
 </sst>
 </file>
@@ -71,17 +87,11 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -89,15 +99,14 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -137,13 +146,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -162,56 +169,150 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Sheets">
+    <a:clrScheme name="Office">
       <a:dk1>
-        <a:srgbClr val="000000"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="FFFFFF"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="000000"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="FFFFFF"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285F4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="EA4335"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="FBBC04"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34A853"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="FF6D01"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46BDC6"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155CC"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Sheets">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial"/>
-        <a:ea typeface="Arial"/>
-        <a:cs typeface="Arial"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -354,159 +455,96 @@
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:N7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC319C0-7BEC-4823-ACDE-B61ED1805D45}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.77734375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="2" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I7" s="1"/>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>